<commit_message>
diretor extraido da planilha
</commit_message>
<xml_diff>
--- a/alunos.xlsx
+++ b/alunos.xlsx
@@ -385,12 +385,15 @@
         <v>nome</v>
       </c>
       <c r="B1" t="str">
-        <v/>
+        <v>diretor</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Carlos Gabriel de Castro Rodrigues</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Gabriel</v>
       </c>
     </row>
     <row r="3">

</xml_diff>